<commit_message>
Finalize models 1 and 2
</commit_message>
<xml_diff>
--- a/sandbox/mike/Resources/cpi.xlsx
+++ b/sandbox/mike/Resources/cpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ardonaghspecialty-my.sharepoint.com/personal/mike_raminski_ardonaghspecialty_onmicrosoft_com/Documents/Desktop/General/UT/__Project_4/UTA_Project-4/sandbox/mike/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{1D2AD301-4D29-48F2-A5A9-DD97CE8FEBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EE7F1DB-1079-4C49-8230-46155015CC87}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{1D2AD301-4D29-48F2-A5A9-DD97CE8FEBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB14791-F8E7-495B-B531-9E03209933B4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF8CF8D2-7568-484E-A90D-010D9E82ACDB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
   <si>
     <t>CPI</t>
   </si>
@@ -213,6 +213,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,9 +516,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BC967F-813B-48B1-B3FD-28682DAD0625}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1871,6 +1877,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="124" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" s="2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>